<commit_message>
add the plugin pattern for multiple bank website connectors add the 1st connector for CM bank update the related unit testing scripts
</commit_message>
<xml_diff>
--- a/perl.xlsx
+++ b/perl.xlsx
@@ -13,28 +13,12 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
-  <si>
-    <t>Hi Excel!</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,11 +44,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,34 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>1.2345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <f>SIN(PI()/4)</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>